<commit_message>
latest changes post QA eecution on VM
</commit_message>
<xml_diff>
--- a/data/BppTrend/Error_Record_Files/BOE Valuation Factors 2020.xlsx
+++ b/data/BppTrend/Error_Record_Files/BOE Valuation Factors 2020.xlsx
@@ -326,14 +326,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -879,7 +879,7 @@
       <c r="B2" s="23">
         <v>61</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="31" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="12"/>
@@ -891,7 +891,7 @@
       <c r="B3" s="23">
         <v>46</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="31" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="12"/>
@@ -1387,30 +1387,30 @@
     </row>
     <row r="22" spans="1:9" ht="15.5">
       <c r="A22" s="7"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
       <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:9" ht="15">
       <c r="A23" s="8"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
       <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:9" ht="14">
       <c r="A24" s="8"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
       <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:9" ht="14">
       <c r="A25" s="9"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="14">
@@ -1892,9 +1892,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2115,19 +2118,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3042FB5-FB08-4B9F-9044-0268488FBE5E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EFFB5BE-0098-48C2-BBB0-46C3FEF9D505}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2152,9 +2151,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EFFB5BE-0098-48C2-BBB0-46C3FEF9D505}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3042FB5-FB08-4B9F-9044-0268488FBE5E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>